<commit_message>
overhaul on feature interactions
Removed all global variables. All methods/functions now return processed/imported data instead of storing them.
Main module created to centralize actions.
</commit_message>
<xml_diff>
--- a/src/defaultipa.xlsx
+++ b/src/defaultipa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\accel\ProjectHome\phonetic-problem-generator\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B5326B-9035-4C59-9B11-4C6D41534206}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5133299A-86BE-4727-B72D-8C928863EC83}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="27977" windowHeight="18120" xr2:uid="{A2B073AC-DFC3-D048-8692-BFCEF974FFF8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="105">
   <si>
     <t>p</t>
   </si>
@@ -99,15 +99,9 @@
     <t>pʰ</t>
   </si>
   <si>
-    <t>aspirated</t>
-  </si>
-  <si>
     <t>bʱ</t>
   </si>
   <si>
-    <t>breathy</t>
-  </si>
-  <si>
     <t>i</t>
   </si>
   <si>
@@ -183,15 +177,6 @@
     <t>dorsal</t>
   </si>
   <si>
-    <t>phonation</t>
-  </si>
-  <si>
-    <t>modal voiced</t>
-  </si>
-  <si>
-    <t>unaspirated voiceless</t>
-  </si>
-  <si>
     <t>vocal fold spread</t>
   </si>
   <si>
@@ -325,15 +310,6 @@
   </si>
   <si>
     <t>specific consonant POA</t>
-  </si>
-  <si>
-    <t>dummy1</t>
-  </si>
-  <si>
-    <t>dummy2</t>
-  </si>
-  <si>
-    <t>dummy3</t>
   </si>
   <si>
     <t>non_syllabic</t>
@@ -715,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{580C24B1-92A6-954F-80C3-690B3863B6C1}">
-  <dimension ref="A2:AH33"/>
+  <dimension ref="A2:AD33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
@@ -745,62 +721,61 @@
     <col min="20" max="20" width="7.5" customWidth="1"/>
     <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="18.640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.45">
       <c r="G2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="I2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="K2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="I3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="K3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="L3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="M3" t="s">
         <v>5</v>
@@ -812,75 +787,63 @@
         <v>10</v>
       </c>
       <c r="P3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Q3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="R3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S3" t="s">
         <v>16</v>
       </c>
       <c r="T3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="U3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="V3" t="s">
-        <v>56</v>
-      </c>
-      <c r="W3" t="s">
-        <v>52</v>
-      </c>
-      <c r="X3" t="s">
-        <v>100</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>101</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M4" t="s">
         <v>6</v>
@@ -892,81 +855,69 @@
         <v>11</v>
       </c>
       <c r="P4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S4" t="s">
         <v>17</v>
       </c>
       <c r="T4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V4" t="s">
-        <v>59</v>
-      </c>
-      <c r="W4" t="s">
         <v>54</v>
       </c>
-      <c r="X4" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>104</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="AB4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M5" t="s">
         <v>7</v>
@@ -978,81 +929,69 @@
         <v>11</v>
       </c>
       <c r="P5" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q5" t="s">
         <v>45</v>
       </c>
-      <c r="Q5" t="s">
-        <v>47</v>
-      </c>
       <c r="R5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S5" t="s">
         <v>17</v>
       </c>
       <c r="T5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="U5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V5" t="s">
-        <v>59</v>
-      </c>
-      <c r="W5" t="s">
         <v>54</v>
       </c>
-      <c r="X5" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>106</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="AB5" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M6" t="s">
         <v>6</v>
@@ -1064,75 +1003,63 @@
         <v>11</v>
       </c>
       <c r="P6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S6" t="s">
         <v>17</v>
       </c>
       <c r="T6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V6" t="s">
-        <v>59</v>
-      </c>
-      <c r="W6" t="s">
-        <v>53</v>
-      </c>
-      <c r="X6" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F7" t="s">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M7" t="s">
         <v>15</v>
@@ -1144,57 +1071,45 @@
         <v>22</v>
       </c>
       <c r="P7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S7" t="s">
         <v>18</v>
       </c>
       <c r="T7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V7" t="s">
-        <v>59</v>
-      </c>
-      <c r="W7" t="s">
-        <v>53</v>
-      </c>
-      <c r="X7" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
         <v>1</v>
@@ -1203,19 +1118,19 @@
         <v>21</v>
       </c>
       <c r="H8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M8" t="s">
         <v>6</v>
@@ -1227,78 +1142,66 @@
         <v>11</v>
       </c>
       <c r="P8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S8" t="s">
         <v>17</v>
       </c>
       <c r="T8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V8" t="s">
-        <v>59</v>
-      </c>
-      <c r="W8" t="s">
         <v>54</v>
       </c>
-      <c r="X8" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="AB8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M10" t="s">
         <v>6</v>
@@ -1310,75 +1213,63 @@
         <v>11</v>
       </c>
       <c r="P10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S10" t="s">
         <v>17</v>
       </c>
       <c r="T10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="V10" t="s">
-        <v>59</v>
-      </c>
-      <c r="W10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="X10" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F11" t="s">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M11" t="s">
         <v>6</v>
@@ -1390,81 +1281,69 @@
         <v>11</v>
       </c>
       <c r="P11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S11" t="s">
         <v>17</v>
       </c>
       <c r="T11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U11" t="s">
+        <v>52</v>
+      </c>
+      <c r="V11" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" t="s">
         <v>57</v>
       </c>
-      <c r="V11" t="s">
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" t="s">
         <v>59</v>
       </c>
-      <c r="W11" t="s">
-        <v>26</v>
-      </c>
-      <c r="X11" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" t="s">
-        <v>78</v>
-      </c>
-      <c r="G13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13" t="s">
-        <v>63</v>
-      </c>
-      <c r="I13" t="s">
-        <v>64</v>
-      </c>
       <c r="J13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M13" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="N13" t="s">
         <v>14</v>
@@ -1473,54 +1352,42 @@
         <v>22</v>
       </c>
       <c r="P13" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q13" t="s">
         <v>45</v>
       </c>
-      <c r="Q13" t="s">
-        <v>47</v>
-      </c>
       <c r="R13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S13" t="s">
         <v>17</v>
       </c>
       <c r="T13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U13" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V13" t="s">
-        <v>59</v>
-      </c>
-      <c r="W13" t="s">
-        <v>53</v>
-      </c>
-      <c r="X13" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F15" t="s">
         <v>1</v>
@@ -1529,22 +1396,22 @@
         <v>21</v>
       </c>
       <c r="H15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J15" t="s">
+        <v>37</v>
+      </c>
+      <c r="K15" t="s">
+        <v>31</v>
+      </c>
+      <c r="L15" t="s">
+        <v>48</v>
+      </c>
+      <c r="M15" t="s">
         <v>39</v>
-      </c>
-      <c r="K15" t="s">
-        <v>33</v>
-      </c>
-      <c r="L15" t="s">
-        <v>50</v>
-      </c>
-      <c r="M15" t="s">
-        <v>41</v>
       </c>
       <c r="N15" t="s">
         <v>14</v>
@@ -1553,75 +1420,63 @@
         <v>22</v>
       </c>
       <c r="P15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S15" t="s">
         <v>17</v>
       </c>
       <c r="T15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U15" t="s">
+        <v>53</v>
+      </c>
+      <c r="V15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" t="s">
         <v>58</v>
       </c>
-      <c r="V15" t="s">
+      <c r="I17" t="s">
         <v>59</v>
       </c>
-      <c r="W15" t="s">
-        <v>53</v>
-      </c>
-      <c r="X15" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" t="s">
-        <v>103</v>
-      </c>
-      <c r="C17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" t="s">
-        <v>78</v>
-      </c>
-      <c r="G17" t="s">
-        <v>50</v>
-      </c>
-      <c r="H17" t="s">
-        <v>63</v>
-      </c>
-      <c r="I17" t="s">
-        <v>64</v>
-      </c>
       <c r="J17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M17" t="s">
         <v>6</v>
@@ -1633,75 +1488,63 @@
         <v>11</v>
       </c>
       <c r="P17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S17" t="s">
         <v>17</v>
       </c>
       <c r="T17" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="U17" t="s">
+        <v>53</v>
+      </c>
+      <c r="V17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" t="s">
         <v>58</v>
       </c>
-      <c r="V17" t="s">
-        <v>59</v>
-      </c>
-      <c r="W17" t="s">
-        <v>54</v>
-      </c>
-      <c r="X17" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" t="s">
-        <v>103</v>
-      </c>
-      <c r="C18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" t="s">
-        <v>79</v>
-      </c>
-      <c r="G18" t="s">
-        <v>50</v>
-      </c>
-      <c r="H18" t="s">
-        <v>63</v>
-      </c>
       <c r="I18" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="J18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M18" t="s">
         <v>7</v>
@@ -1713,75 +1556,63 @@
         <v>11</v>
       </c>
       <c r="P18" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q18" t="s">
         <v>45</v>
       </c>
-      <c r="Q18" t="s">
-        <v>47</v>
-      </c>
       <c r="R18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S18" t="s">
         <v>17</v>
       </c>
       <c r="T18" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="U18" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V18" t="s">
-        <v>59</v>
-      </c>
-      <c r="W18" t="s">
         <v>54</v>
       </c>
-      <c r="X18" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F19" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H19" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I19" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="J19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M19" t="s">
         <v>7</v>
@@ -1793,75 +1624,63 @@
         <v>11</v>
       </c>
       <c r="P19" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q19" t="s">
         <v>45</v>
       </c>
-      <c r="Q19" t="s">
-        <v>47</v>
-      </c>
       <c r="R19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S19" t="s">
         <v>17</v>
       </c>
       <c r="T19" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="U19" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" t="s">
+        <v>66</v>
+      </c>
+      <c r="I20" t="s">
         <v>59</v>
       </c>
-      <c r="W19" t="s">
-        <v>54</v>
-      </c>
-      <c r="X19" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" t="s">
-        <v>103</v>
-      </c>
-      <c r="C20" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20" t="s">
-        <v>81</v>
-      </c>
-      <c r="G20" t="s">
-        <v>50</v>
-      </c>
-      <c r="H20" t="s">
-        <v>71</v>
-      </c>
-      <c r="I20" t="s">
-        <v>64</v>
-      </c>
       <c r="J20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M20" t="s">
         <v>7</v>
@@ -1873,75 +1692,63 @@
         <v>11</v>
       </c>
       <c r="P20" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q20" t="s">
         <v>45</v>
       </c>
-      <c r="Q20" t="s">
-        <v>47</v>
-      </c>
       <c r="R20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S20" t="s">
         <v>17</v>
       </c>
       <c r="T20" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="U20" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V20" t="s">
-        <v>59</v>
-      </c>
-      <c r="W20" t="s">
         <v>54</v>
       </c>
-      <c r="X20" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F22" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M22" t="s">
         <v>7</v>
@@ -1953,75 +1760,63 @@
         <v>11</v>
       </c>
       <c r="P22" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q22" t="s">
         <v>45</v>
       </c>
-      <c r="Q22" t="s">
-        <v>47</v>
-      </c>
       <c r="R22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S22" t="s">
         <v>17</v>
       </c>
       <c r="T22" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="U22" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="V22" t="s">
-        <v>59</v>
-      </c>
-      <c r="W22" t="s">
-        <v>24</v>
-      </c>
-      <c r="X22" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F23" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M23" t="s">
         <v>6</v>
@@ -2033,78 +1828,66 @@
         <v>11</v>
       </c>
       <c r="P23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S23" t="s">
         <v>17</v>
       </c>
       <c r="T23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U23" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V23" t="s">
-        <v>90</v>
-      </c>
-      <c r="W23" t="s">
-        <v>54</v>
-      </c>
-      <c r="X23" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.45">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D25" t="s">
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H25" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I25" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="J25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L25" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="M25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N25" t="s">
         <v>14</v>
@@ -2113,78 +1896,66 @@
         <v>22</v>
       </c>
       <c r="P25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S25" t="s">
         <v>17</v>
       </c>
       <c r="T25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U25" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V25" t="s">
-        <v>59</v>
-      </c>
-      <c r="W25" t="s">
-        <v>53</v>
-      </c>
-      <c r="X25" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D26" t="s">
         <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H26" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I26" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="J26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L26" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="M26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N26" t="s">
         <v>14</v>
@@ -2193,78 +1964,66 @@
         <v>22</v>
       </c>
       <c r="P26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S26" t="s">
         <v>17</v>
       </c>
       <c r="T26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U26" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V26" t="s">
-        <v>59</v>
-      </c>
-      <c r="W26" t="s">
-        <v>53</v>
-      </c>
-      <c r="X26" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z26" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D27" t="s">
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H27" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I27" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="J27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L27" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="M27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N27" t="s">
         <v>14</v>
@@ -2273,78 +2032,66 @@
         <v>22</v>
       </c>
       <c r="P27" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S27" t="s">
         <v>17</v>
       </c>
       <c r="T27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U27" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V27" t="s">
-        <v>59</v>
-      </c>
-      <c r="W27" t="s">
-        <v>53</v>
-      </c>
-      <c r="X27" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D28" t="s">
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H28" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I28" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="J28" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L28" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="M28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N28" t="s">
         <v>14</v>
@@ -2353,78 +2100,66 @@
         <v>22</v>
       </c>
       <c r="P28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S28" t="s">
         <v>17</v>
       </c>
       <c r="T28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U28" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V28" t="s">
-        <v>59</v>
-      </c>
-      <c r="W28" t="s">
-        <v>53</v>
-      </c>
-      <c r="X28" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y28" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z28" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D29" t="s">
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G29" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" t="s">
+        <v>48</v>
+      </c>
+      <c r="J29" t="s">
         <v>36</v>
       </c>
-      <c r="H29" t="s">
-        <v>50</v>
-      </c>
-      <c r="I29" t="s">
-        <v>50</v>
-      </c>
-      <c r="J29" t="s">
-        <v>38</v>
-      </c>
       <c r="K29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L29" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="M29" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N29" t="s">
         <v>14</v>
@@ -2433,78 +2168,66 @@
         <v>22</v>
       </c>
       <c r="P29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S29" t="s">
         <v>17</v>
       </c>
       <c r="T29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U29" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V29" t="s">
-        <v>59</v>
-      </c>
-      <c r="W29" t="s">
-        <v>53</v>
-      </c>
-      <c r="X29" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D30" t="s">
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G30" t="s">
         <v>21</v>
       </c>
       <c r="H30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K30" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="L30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="M30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N30" t="s">
         <v>14</v>
@@ -2513,78 +2236,66 @@
         <v>22</v>
       </c>
       <c r="P30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S30" t="s">
         <v>17</v>
       </c>
       <c r="T30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U30" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V30" t="s">
-        <v>59</v>
-      </c>
-      <c r="W30" t="s">
-        <v>53</v>
-      </c>
-      <c r="X30" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y30" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z30" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D31" t="s">
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G31" t="s">
         <v>21</v>
       </c>
       <c r="H31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L31" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="M31" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N31" t="s">
         <v>14</v>
@@ -2593,75 +2304,63 @@
         <v>22</v>
       </c>
       <c r="P31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S31" t="s">
         <v>17</v>
       </c>
       <c r="T31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U31" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V31" t="s">
-        <v>59</v>
-      </c>
-      <c r="W31" t="s">
-        <v>53</v>
-      </c>
-      <c r="X31" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y31" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B33" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F33" t="s">
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M33" t="s">
         <v>15</v>
@@ -2673,37 +2372,25 @@
         <v>22</v>
       </c>
       <c r="P33" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S33" t="s">
         <v>18</v>
       </c>
       <c r="T33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U33" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V33" t="s">
-        <v>59</v>
-      </c>
-      <c r="W33" t="s">
         <v>54</v>
-      </c>
-      <c r="X33" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y33" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z33" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Template functions & format change
Disallow any special characters else than space in descriptions of features
Disallow using space as seperator in any forms of conjuction between particles/features in external files
Function for generating sound list matching given particle
</commit_message>
<xml_diff>
--- a/src/defaultipa.xlsx
+++ b/src/defaultipa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\accel\ProjectHome\phonetic-problem-generator\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5133299A-86BE-4727-B72D-8C928863EC83}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B75B5EE-3CE2-4984-A2AE-5644DCF53109}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="27977" windowHeight="18120" xr2:uid="{A2B073AC-DFC3-D048-8692-BFCEF974FFF8}"/>
   </bookViews>
@@ -312,9 +312,6 @@
     <t>specific consonant POA</t>
   </si>
   <si>
-    <t>non_syllabic</t>
-  </si>
-  <si>
     <t>bilabial _&gt; labial</t>
   </si>
   <si>
@@ -340,6 +337,9 @@
   </si>
   <si>
     <t>middle</t>
+  </si>
+  <si>
+    <t>non syllabic</t>
   </si>
 </sst>
 </file>
@@ -693,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{580C24B1-92A6-954F-80C3-690B3863B6C1}">
   <dimension ref="A2:AD33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="Y11" sqref="Y11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
@@ -742,7 +742,7 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
         <v>55</v>
@@ -813,7 +813,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -876,10 +876,10 @@
         <v>54</v>
       </c>
       <c r="AB4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD4" t="s">
         <v>96</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.45">
@@ -887,7 +887,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -950,10 +950,10 @@
         <v>54</v>
       </c>
       <c r="AB5" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD5" t="s">
         <v>98</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.45">
@@ -961,7 +961,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -1029,7 +1029,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -1092,7 +1092,7 @@
         <v>54</v>
       </c>
       <c r="AB7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.45">
@@ -1100,7 +1100,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1163,7 +1163,7 @@
         <v>54</v>
       </c>
       <c r="AB8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.45">
@@ -1171,7 +1171,7 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -1239,7 +1239,7 @@
         <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1302,7 +1302,7 @@
         <v>54</v>
       </c>
       <c r="AB11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.45">
@@ -1310,7 +1310,7 @@
         <v>86</v>
       </c>
       <c r="B13" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C13" t="s">
         <v>57</v>
@@ -1378,7 +1378,7 @@
         <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -1446,7 +1446,7 @@
         <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C17" t="s">
         <v>57</v>
@@ -1514,7 +1514,7 @@
         <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C18" t="s">
         <v>57</v>
@@ -1582,7 +1582,7 @@
         <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C19" t="s">
         <v>57</v>
@@ -1650,7 +1650,7 @@
         <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C20" t="s">
         <v>57</v>
@@ -1718,7 +1718,7 @@
         <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C22" t="s">
         <v>48</v>
@@ -1786,7 +1786,7 @@
         <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C23" t="s">
         <v>48</v>
@@ -2221,7 +2221,7 @@
         <v>37</v>
       </c>
       <c r="K30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L30" t="s">
         <v>80</v>
@@ -2330,7 +2330,7 @@
         <v>81</v>
       </c>
       <c r="B33" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>

</xml_diff>